<commit_message>
finish task1: mean and polynomial
</commit_message>
<xml_diff>
--- a/code/lake_data/completeChinaLake.xlsx
+++ b/code/lake_data/completeChinaLake.xlsx
@@ -1626,7 +1626,7 @@
         <v>7</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.008799999999999997</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>9.699999999999999</v>
@@ -1663,7 +1663,7 @@
         <v>7</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.001999999999999998</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>16.25</v>
@@ -3180,7 +3180,7 @@
         <v>7</v>
       </c>
       <c r="G74" t="n">
-        <v>-0.022</v>
+        <v>0</v>
       </c>
       <c r="H74" t="n">
         <v>10.9</v>
@@ -3918,7 +3918,7 @@
         <v>13.3</v>
       </c>
       <c r="I2" t="n">
-        <v>0.014</v>
+        <v>0.01381250000000006</v>
       </c>
     </row>
     <row r="3">
@@ -4097,13 +4097,13 @@
         <v>7</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03488999999999999</v>
+        <v>0.027003</v>
       </c>
       <c r="H7" t="n">
-        <v>17.36666666666666</v>
+        <v>18.10999999999986</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02150000000000001</v>
+        <v>0.02443750000000008</v>
       </c>
     </row>
     <row r="8">
@@ -4282,7 +4282,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="n">
-        <v>0.02435499999999999</v>
+        <v>0.004392499999999994</v>
       </c>
       <c r="H12" t="n">
         <v>18.8</v>
@@ -4319,7 +4319,7 @@
         <v>7</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03281999999999999</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>14.3</v>
@@ -4578,13 +4578,13 @@
         <v>7</v>
       </c>
       <c r="G20" t="n">
-        <v>0.003700000000000001</v>
+        <v>0.002000000000000005</v>
       </c>
       <c r="H20" t="n">
         <v>11.9</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02166666666666667</v>
+        <v>0.02333333333333341</v>
       </c>
     </row>
     <row r="21">
@@ -4763,13 +4763,13 @@
         <v>7</v>
       </c>
       <c r="G25" t="n">
-        <v>0.00775</v>
+        <v>0.018975</v>
       </c>
       <c r="H25" t="n">
         <v>15.1</v>
       </c>
       <c r="I25" t="n">
-        <v>0.01866666666666667</v>
+        <v>0.02233333333333345</v>
       </c>
     </row>
     <row r="26">
@@ -5022,13 +5022,13 @@
         <v>7</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.008799999999999997</v>
+        <v>0.0006300000000000056</v>
       </c>
       <c r="H32" t="n">
         <v>9.699999999999999</v>
       </c>
       <c r="I32" t="n">
-        <v>0.01025</v>
+        <v>0.01346666666666666</v>
       </c>
     </row>
     <row r="33">
@@ -5059,7 +5059,7 @@
         <v>7</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.001999999999999998</v>
+        <v>0.00375000000000001</v>
       </c>
       <c r="H33" t="n">
         <v>16.25</v>
@@ -5614,13 +5614,13 @@
         <v>7</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0225</v>
+        <v>0.0189560810810811</v>
       </c>
       <c r="H48" t="n">
-        <v>18.175</v>
+        <v>18.97474226804133</v>
       </c>
       <c r="I48" t="n">
-        <v>0.018875</v>
+        <v>0.01930670103092786</v>
       </c>
     </row>
     <row r="49">
@@ -5876,7 +5876,7 @@
         <v>0.022</v>
       </c>
       <c r="H55" t="n">
-        <v>21.6</v>
+        <v>19.62999999999992</v>
       </c>
       <c r="I55" t="n">
         <v>0.02075</v>
@@ -5913,7 +5913,7 @@
         <v>0.02100333333333333</v>
       </c>
       <c r="H56" t="n">
-        <v>12.2</v>
+        <v>11.44999999999993</v>
       </c>
       <c r="I56" t="n">
         <v>0.02733333333333333</v>
@@ -6098,7 +6098,7 @@
         <v>0.018</v>
       </c>
       <c r="H61" t="n">
-        <v>21.65</v>
+        <v>17.59999999999989</v>
       </c>
       <c r="I61" t="n">
         <v>0.018</v>
@@ -6539,13 +6539,13 @@
         <v>7</v>
       </c>
       <c r="G73" t="n">
-        <v>0.012</v>
+        <v>0.02830333333333334</v>
       </c>
       <c r="H73" t="n">
         <v>11.9</v>
       </c>
       <c r="I73" t="n">
-        <v>0.0274</v>
+        <v>0.02897333333333342</v>
       </c>
     </row>
     <row r="74">
@@ -6576,7 +6576,7 @@
         <v>7</v>
       </c>
       <c r="G74" t="n">
-        <v>-0.022</v>
+        <v>0.02046666666666667</v>
       </c>
       <c r="H74" t="n">
         <v>10.9</v>
@@ -6767,7 +6767,7 @@
         <v>16.7</v>
       </c>
       <c r="I79" t="n">
-        <v>0.0215</v>
+        <v>0.02330000000000004</v>
       </c>
     </row>
     <row r="80">
@@ -6909,13 +6909,13 @@
         <v>7</v>
       </c>
       <c r="G83" t="n">
-        <v>0.0146</v>
+        <v>0.01233392857142857</v>
       </c>
       <c r="H83" t="n">
-        <v>19.6</v>
+        <v>20.20909090909084</v>
       </c>
       <c r="I83" t="n">
-        <v>0.01825</v>
+        <v>0.01875000000000001</v>
       </c>
     </row>
     <row r="84">
@@ -6946,7 +6946,7 @@
         <v>7</v>
       </c>
       <c r="G84" t="n">
-        <v>0.01405</v>
+        <v>0.01340535714285715</v>
       </c>
       <c r="H84" t="n">
         <v>21.4</v>
@@ -7094,13 +7094,13 @@
         <v>7</v>
       </c>
       <c r="G88" t="n">
-        <v>0.0185</v>
+        <v>0.01498837209302324</v>
       </c>
       <c r="H88" t="n">
         <v>16.8</v>
       </c>
       <c r="I88" t="n">
-        <v>0.018875</v>
+        <v>0.01936363636363636</v>
       </c>
     </row>
     <row r="89">

</xml_diff>

<commit_message>
finish task1 and task2
</commit_message>
<xml_diff>
--- a/code/lake_data/completeChinaLake.xlsx
+++ b/code/lake_data/completeChinaLake.xlsx
@@ -553,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="n">
-        <v>0.004889999999999999</v>
+        <v>0.00489</v>
       </c>
       <c r="H3" t="n">
         <v>16.55</v>
@@ -630,7 +630,7 @@
         <v>0.01531</v>
       </c>
       <c r="H5" t="n">
-        <v>22.16666666666667</v>
+        <v>22.166667</v>
       </c>
       <c r="I5" t="n">
         <v>0.017</v>
@@ -667,7 +667,7 @@
         <v>0.0251</v>
       </c>
       <c r="H6" t="n">
-        <v>19.76666666666667</v>
+        <v>19.766667</v>
       </c>
       <c r="I6" t="n">
         <v>0.01925</v>
@@ -701,13 +701,13 @@
         <v>7</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03488999999999999</v>
+        <v>0.03489</v>
       </c>
       <c r="H7" t="n">
-        <v>17.36666666666666</v>
+        <v>17.366667</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02150000000000001</v>
+        <v>0.0215</v>
       </c>
     </row>
     <row r="8">
@@ -775,7 +775,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03744500000000001</v>
+        <v>0.037445</v>
       </c>
       <c r="H9" t="n">
         <v>17.2</v>
@@ -852,10 +852,10 @@
         <v>0.01589</v>
       </c>
       <c r="H11" t="n">
-        <v>20.03333333333333</v>
+        <v>20.033333</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01966666666666667</v>
+        <v>0.019667</v>
       </c>
     </row>
     <row r="12">
@@ -886,7 +886,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="n">
-        <v>0.02435499999999999</v>
+        <v>0.024355</v>
       </c>
       <c r="H12" t="n">
         <v>18.8</v>
@@ -923,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03281999999999999</v>
+        <v>0.03282</v>
       </c>
       <c r="H13" t="n">
         <v>14.3</v>
@@ -1003,7 +1003,7 @@
         <v>16.45</v>
       </c>
       <c r="I15" t="n">
-        <v>0.01733333333333334</v>
+        <v>0.017333</v>
       </c>
     </row>
     <row r="16">
@@ -1074,10 +1074,10 @@
         <v>0.0207</v>
       </c>
       <c r="H17" t="n">
-        <v>20.73333333333333</v>
+        <v>20.733333</v>
       </c>
       <c r="I17" t="n">
-        <v>0.01633333333333334</v>
+        <v>0.016333</v>
       </c>
     </row>
     <row r="18">
@@ -1182,13 +1182,13 @@
         <v>7</v>
       </c>
       <c r="G20" t="n">
-        <v>0.003700000000000001</v>
+        <v>0.0037</v>
       </c>
       <c r="H20" t="n">
         <v>11.9</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02166666666666667</v>
+        <v>0.021667</v>
       </c>
     </row>
     <row r="21">
@@ -1259,10 +1259,10 @@
         <v>0.0065</v>
       </c>
       <c r="H22" t="n">
-        <v>18.76666666666667</v>
+        <v>18.766667</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01433333333333334</v>
+        <v>0.014333</v>
       </c>
     </row>
     <row r="23">
@@ -1299,7 +1299,7 @@
         <v>20.15</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01533333333333333</v>
+        <v>0.015333</v>
       </c>
     </row>
     <row r="24">
@@ -1373,7 +1373,7 @@
         <v>15.1</v>
       </c>
       <c r="I25" t="n">
-        <v>0.01866666666666667</v>
+        <v>0.018667</v>
       </c>
     </row>
     <row r="26">
@@ -1447,7 +1447,7 @@
         <v>15.45</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01433333333333333</v>
+        <v>0.014333</v>
       </c>
     </row>
     <row r="28">
@@ -1558,7 +1558,7 @@
         <v>19.8</v>
       </c>
       <c r="I30" t="n">
-        <v>0.01833333333333334</v>
+        <v>0.018333</v>
       </c>
     </row>
     <row r="31">
@@ -1595,7 +1595,7 @@
         <v>16.35</v>
       </c>
       <c r="I31" t="n">
-        <v>0.02133333333333333</v>
+        <v>0.021333</v>
       </c>
     </row>
     <row r="32">
@@ -1743,7 +1743,7 @@
         <v>20.2</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01466666666666667</v>
+        <v>0.014667</v>
       </c>
     </row>
     <row r="36">
@@ -1848,7 +1848,7 @@
         <v>7</v>
       </c>
       <c r="G38" t="n">
-        <v>0.006900000000000001</v>
+        <v>0.0069</v>
       </c>
       <c r="H38" t="n">
         <v>9.9</v>
@@ -1885,10 +1885,10 @@
         <v>7</v>
       </c>
       <c r="G39" t="n">
-        <v>0.004933333333333334</v>
+        <v>0.004933</v>
       </c>
       <c r="H39" t="n">
-        <v>11.26666666666667</v>
+        <v>11.266667</v>
       </c>
       <c r="I39" t="n">
         <v>0.02</v>
@@ -2292,7 +2292,7 @@
         <v>7</v>
       </c>
       <c r="G50" t="n">
-        <v>0.006900000000000001</v>
+        <v>0.0069</v>
       </c>
       <c r="H50" t="n">
         <v>9.85</v>
@@ -2514,13 +2514,13 @@
         <v>7</v>
       </c>
       <c r="G56" t="n">
-        <v>0.02100333333333333</v>
+        <v>0.021003</v>
       </c>
       <c r="H56" t="n">
         <v>12.2</v>
       </c>
       <c r="I56" t="n">
-        <v>0.02733333333333333</v>
+        <v>0.027333</v>
       </c>
     </row>
     <row r="57">
@@ -2662,7 +2662,7 @@
         <v>7</v>
       </c>
       <c r="G60" t="n">
-        <v>0.01533333333333333</v>
+        <v>0.015333</v>
       </c>
       <c r="H60" t="n">
         <v>21.5</v>
@@ -2813,7 +2813,7 @@
         <v>0.01102</v>
       </c>
       <c r="H64" t="n">
-        <v>18.62857142857143</v>
+        <v>18.628571</v>
       </c>
       <c r="I64" t="n">
         <v>0.0171</v>
@@ -2853,7 +2853,7 @@
         <v>21</v>
       </c>
       <c r="I65" t="n">
-        <v>0.01471428571428572</v>
+        <v>0.014714</v>
       </c>
     </row>
     <row r="66">
@@ -2958,7 +2958,7 @@
         <v>7</v>
       </c>
       <c r="G68" t="n">
-        <v>0.003666666666666667</v>
+        <v>0.003667</v>
       </c>
       <c r="H68" t="n">
         <v>13.4</v>
@@ -2998,7 +2998,7 @@
         <v>0.0037</v>
       </c>
       <c r="H69" t="n">
-        <v>17.73333333333333</v>
+        <v>17.733333</v>
       </c>
       <c r="I69" t="n">
         <v>0.0156</v>
@@ -3038,7 +3038,7 @@
         <v>21.525</v>
       </c>
       <c r="I70" t="n">
-        <v>0.01433333333333333</v>
+        <v>0.014333</v>
       </c>
     </row>
     <row r="71">
@@ -3328,10 +3328,10 @@
         <v>7</v>
       </c>
       <c r="G78" t="n">
-        <v>0.03033333333333333</v>
+        <v>0.030333</v>
       </c>
       <c r="H78" t="n">
-        <v>19.93333333333333</v>
+        <v>19.933333</v>
       </c>
       <c r="I78" t="n">
         <v>0.02025</v>
@@ -3918,7 +3918,7 @@
         <v>13.3</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01381250000000006</v>
+        <v>0.013813</v>
       </c>
     </row>
     <row r="3">
@@ -3949,7 +3949,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="n">
-        <v>0.004889999999999999</v>
+        <v>0.00489</v>
       </c>
       <c r="H3" t="n">
         <v>16.55</v>
@@ -4026,7 +4026,7 @@
         <v>0.01531</v>
       </c>
       <c r="H5" t="n">
-        <v>22.16666666666667</v>
+        <v>22.166667</v>
       </c>
       <c r="I5" t="n">
         <v>0.017</v>
@@ -4063,7 +4063,7 @@
         <v>0.0251</v>
       </c>
       <c r="H6" t="n">
-        <v>19.76666666666667</v>
+        <v>19.766667</v>
       </c>
       <c r="I6" t="n">
         <v>0.01925</v>
@@ -4100,10 +4100,10 @@
         <v>0.027003</v>
       </c>
       <c r="H7" t="n">
-        <v>18.10999999999986</v>
+        <v>18.11</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02443750000000008</v>
+        <v>0.024438</v>
       </c>
     </row>
     <row r="8">
@@ -4171,7 +4171,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03744500000000001</v>
+        <v>0.037445</v>
       </c>
       <c r="H9" t="n">
         <v>17.2</v>
@@ -4248,10 +4248,10 @@
         <v>0.01589</v>
       </c>
       <c r="H11" t="n">
-        <v>20.03333333333333</v>
+        <v>20.033333</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01966666666666667</v>
+        <v>0.019667</v>
       </c>
     </row>
     <row r="12">
@@ -4282,7 +4282,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="n">
-        <v>0.004392499999999994</v>
+        <v>0.004392</v>
       </c>
       <c r="H12" t="n">
         <v>18.8</v>
@@ -4399,7 +4399,7 @@
         <v>16.45</v>
       </c>
       <c r="I15" t="n">
-        <v>0.01733333333333334</v>
+        <v>0.017333</v>
       </c>
     </row>
     <row r="16">
@@ -4470,10 +4470,10 @@
         <v>0.0207</v>
       </c>
       <c r="H17" t="n">
-        <v>20.73333333333333</v>
+        <v>20.733333</v>
       </c>
       <c r="I17" t="n">
-        <v>0.01633333333333334</v>
+        <v>0.016333</v>
       </c>
     </row>
     <row r="18">
@@ -4578,13 +4578,13 @@
         <v>7</v>
       </c>
       <c r="G20" t="n">
-        <v>0.002000000000000005</v>
+        <v>0.002</v>
       </c>
       <c r="H20" t="n">
         <v>11.9</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02333333333333341</v>
+        <v>0.023333</v>
       </c>
     </row>
     <row r="21">
@@ -4655,10 +4655,10 @@
         <v>0.0065</v>
       </c>
       <c r="H22" t="n">
-        <v>18.76666666666667</v>
+        <v>18.766667</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01433333333333334</v>
+        <v>0.014333</v>
       </c>
     </row>
     <row r="23">
@@ -4695,7 +4695,7 @@
         <v>20.15</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01533333333333333</v>
+        <v>0.015333</v>
       </c>
     </row>
     <row r="24">
@@ -4769,7 +4769,7 @@
         <v>15.1</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02233333333333345</v>
+        <v>0.022333</v>
       </c>
     </row>
     <row r="26">
@@ -4843,7 +4843,7 @@
         <v>15.45</v>
       </c>
       <c r="I27" t="n">
-        <v>0.01433333333333333</v>
+        <v>0.014333</v>
       </c>
     </row>
     <row r="28">
@@ -4954,7 +4954,7 @@
         <v>19.8</v>
       </c>
       <c r="I30" t="n">
-        <v>0.01833333333333334</v>
+        <v>0.018333</v>
       </c>
     </row>
     <row r="31">
@@ -4991,7 +4991,7 @@
         <v>16.35</v>
       </c>
       <c r="I31" t="n">
-        <v>0.02133333333333333</v>
+        <v>0.021333</v>
       </c>
     </row>
     <row r="32">
@@ -5022,13 +5022,13 @@
         <v>7</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0006300000000000056</v>
+        <v>0.00063</v>
       </c>
       <c r="H32" t="n">
         <v>9.699999999999999</v>
       </c>
       <c r="I32" t="n">
-        <v>0.01346666666666666</v>
+        <v>0.013467</v>
       </c>
     </row>
     <row r="33">
@@ -5059,7 +5059,7 @@
         <v>7</v>
       </c>
       <c r="G33" t="n">
-        <v>0.00375000000000001</v>
+        <v>0.00375</v>
       </c>
       <c r="H33" t="n">
         <v>16.25</v>
@@ -5139,7 +5139,7 @@
         <v>20.2</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01466666666666667</v>
+        <v>0.014667</v>
       </c>
     </row>
     <row r="36">
@@ -5244,7 +5244,7 @@
         <v>7</v>
       </c>
       <c r="G38" t="n">
-        <v>0.006900000000000001</v>
+        <v>0.0069</v>
       </c>
       <c r="H38" t="n">
         <v>9.9</v>
@@ -5281,10 +5281,10 @@
         <v>7</v>
       </c>
       <c r="G39" t="n">
-        <v>0.004933333333333334</v>
+        <v>0.004933</v>
       </c>
       <c r="H39" t="n">
-        <v>11.26666666666667</v>
+        <v>11.266667</v>
       </c>
       <c r="I39" t="n">
         <v>0.02</v>
@@ -5614,13 +5614,13 @@
         <v>7</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0189560810810811</v>
+        <v>0.018956</v>
       </c>
       <c r="H48" t="n">
-        <v>18.97474226804133</v>
+        <v>18.974742</v>
       </c>
       <c r="I48" t="n">
-        <v>0.01930670103092786</v>
+        <v>0.019307</v>
       </c>
     </row>
     <row r="49">
@@ -5688,7 +5688,7 @@
         <v>7</v>
       </c>
       <c r="G50" t="n">
-        <v>0.006900000000000001</v>
+        <v>0.0069</v>
       </c>
       <c r="H50" t="n">
         <v>9.85</v>
@@ -5876,7 +5876,7 @@
         <v>0.022</v>
       </c>
       <c r="H55" t="n">
-        <v>19.62999999999992</v>
+        <v>19.63</v>
       </c>
       <c r="I55" t="n">
         <v>0.02075</v>
@@ -5910,13 +5910,13 @@
         <v>7</v>
       </c>
       <c r="G56" t="n">
-        <v>0.02100333333333333</v>
+        <v>0.021003</v>
       </c>
       <c r="H56" t="n">
-        <v>11.44999999999993</v>
+        <v>11.45</v>
       </c>
       <c r="I56" t="n">
-        <v>0.02733333333333333</v>
+        <v>0.027333</v>
       </c>
     </row>
     <row r="57">
@@ -6058,7 +6058,7 @@
         <v>7</v>
       </c>
       <c r="G60" t="n">
-        <v>0.01533333333333333</v>
+        <v>0.015333</v>
       </c>
       <c r="H60" t="n">
         <v>21.5</v>
@@ -6098,7 +6098,7 @@
         <v>0.018</v>
       </c>
       <c r="H61" t="n">
-        <v>17.59999999999989</v>
+        <v>17.6</v>
       </c>
       <c r="I61" t="n">
         <v>0.018</v>
@@ -6209,7 +6209,7 @@
         <v>0.01102</v>
       </c>
       <c r="H64" t="n">
-        <v>18.62857142857143</v>
+        <v>18.628571</v>
       </c>
       <c r="I64" t="n">
         <v>0.0171</v>
@@ -6249,7 +6249,7 @@
         <v>21</v>
       </c>
       <c r="I65" t="n">
-        <v>0.01471428571428572</v>
+        <v>0.014714</v>
       </c>
     </row>
     <row r="66">
@@ -6354,7 +6354,7 @@
         <v>7</v>
       </c>
       <c r="G68" t="n">
-        <v>0.003666666666666667</v>
+        <v>0.003667</v>
       </c>
       <c r="H68" t="n">
         <v>13.4</v>
@@ -6394,7 +6394,7 @@
         <v>0.0037</v>
       </c>
       <c r="H69" t="n">
-        <v>17.73333333333333</v>
+        <v>17.733333</v>
       </c>
       <c r="I69" t="n">
         <v>0.0156</v>
@@ -6434,7 +6434,7 @@
         <v>21.525</v>
       </c>
       <c r="I70" t="n">
-        <v>0.01433333333333333</v>
+        <v>0.014333</v>
       </c>
     </row>
     <row r="71">
@@ -6539,13 +6539,13 @@
         <v>7</v>
       </c>
       <c r="G73" t="n">
-        <v>0.02830333333333334</v>
+        <v>0.028303</v>
       </c>
       <c r="H73" t="n">
         <v>11.9</v>
       </c>
       <c r="I73" t="n">
-        <v>0.02897333333333342</v>
+        <v>0.028973</v>
       </c>
     </row>
     <row r="74">
@@ -6576,7 +6576,7 @@
         <v>7</v>
       </c>
       <c r="G74" t="n">
-        <v>0.02046666666666667</v>
+        <v>0.020467</v>
       </c>
       <c r="H74" t="n">
         <v>10.9</v>
@@ -6724,10 +6724,10 @@
         <v>7</v>
       </c>
       <c r="G78" t="n">
-        <v>0.03033333333333333</v>
+        <v>0.030333</v>
       </c>
       <c r="H78" t="n">
-        <v>19.93333333333333</v>
+        <v>19.933333</v>
       </c>
       <c r="I78" t="n">
         <v>0.02025</v>
@@ -6767,7 +6767,7 @@
         <v>16.7</v>
       </c>
       <c r="I79" t="n">
-        <v>0.02330000000000004</v>
+        <v>0.0233</v>
       </c>
     </row>
     <row r="80">
@@ -6909,13 +6909,13 @@
         <v>7</v>
       </c>
       <c r="G83" t="n">
-        <v>0.01233392857142857</v>
+        <v>0.012334</v>
       </c>
       <c r="H83" t="n">
-        <v>20.20909090909084</v>
+        <v>20.209091</v>
       </c>
       <c r="I83" t="n">
-        <v>0.01875000000000001</v>
+        <v>0.01875</v>
       </c>
     </row>
     <row r="84">
@@ -6946,7 +6946,7 @@
         <v>7</v>
       </c>
       <c r="G84" t="n">
-        <v>0.01340535714285715</v>
+        <v>0.013405</v>
       </c>
       <c r="H84" t="n">
         <v>21.4</v>
@@ -7094,13 +7094,13 @@
         <v>7</v>
       </c>
       <c r="G88" t="n">
-        <v>0.01498837209302324</v>
+        <v>0.014988</v>
       </c>
       <c r="H88" t="n">
         <v>16.8</v>
       </c>
       <c r="I88" t="n">
-        <v>0.01936363636363636</v>
+        <v>0.019364</v>
       </c>
     </row>
     <row r="89">

</xml_diff>

<commit_message>
update best match priority
</commit_message>
<xml_diff>
--- a/code/lake_data/completeChinaLake.xlsx
+++ b/code/lake_data/completeChinaLake.xlsx
@@ -556,7 +556,7 @@
         <v>0.00489</v>
       </c>
       <c r="H3" t="n">
-        <v>16.55</v>
+        <v>17.7</v>
       </c>
       <c r="I3" t="n">
         <v>0.0135</v>
@@ -630,7 +630,7 @@
         <v>0.01531</v>
       </c>
       <c r="H5" t="n">
-        <v>22.166667</v>
+        <v>21.5</v>
       </c>
       <c r="I5" t="n">
         <v>0.017</v>
@@ -667,7 +667,7 @@
         <v>0.0251</v>
       </c>
       <c r="H6" t="n">
-        <v>19.766667</v>
+        <v>20.8</v>
       </c>
       <c r="I6" t="n">
         <v>0.01925</v>
@@ -704,7 +704,7 @@
         <v>0.03489</v>
       </c>
       <c r="H7" t="n">
-        <v>17.366667</v>
+        <v>20.1</v>
       </c>
       <c r="I7" t="n">
         <v>0.0215</v>
@@ -812,13 +812,13 @@
         <v>7</v>
       </c>
       <c r="G10" t="n">
-        <v>0.007425</v>
+        <v>0.00625</v>
       </c>
       <c r="H10" t="n">
         <v>20.3</v>
       </c>
       <c r="I10" t="n">
-        <v>0.019</v>
+        <v>0.0185</v>
       </c>
     </row>
     <row r="11">
@@ -849,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01589</v>
+        <v>0.015887</v>
       </c>
       <c r="H11" t="n">
         <v>20.033333</v>
@@ -886,7 +886,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="n">
-        <v>0.024355</v>
+        <v>0.025523</v>
       </c>
       <c r="H12" t="n">
         <v>18.8</v>
@@ -923,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03282</v>
+        <v>0.03516</v>
       </c>
       <c r="H13" t="n">
         <v>14.3</v>
@@ -963,10 +963,10 @@
         <v>0.007</v>
       </c>
       <c r="H14" t="n">
-        <v>12.25</v>
+        <v>13.5</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01975</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="15">
@@ -1000,10 +1000,10 @@
         <v>0.0046</v>
       </c>
       <c r="H15" t="n">
-        <v>16.45</v>
+        <v>18.1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.017333</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="16">
@@ -1074,7 +1074,7 @@
         <v>0.0207</v>
       </c>
       <c r="H17" t="n">
-        <v>20.733333</v>
+        <v>20.5</v>
       </c>
       <c r="I17" t="n">
         <v>0.016333</v>
@@ -1333,7 +1333,7 @@
         <v>0.0127</v>
       </c>
       <c r="H24" t="n">
-        <v>19.65</v>
+        <v>18.8</v>
       </c>
       <c r="I24" t="n">
         <v>0.017</v>
@@ -1555,10 +1555,10 @@
         <v>0.0318</v>
       </c>
       <c r="H30" t="n">
-        <v>19.8</v>
+        <v>20.4</v>
       </c>
       <c r="I30" t="n">
-        <v>0.018333</v>
+        <v>0.0185</v>
       </c>
     </row>
     <row r="31">
@@ -1592,10 +1592,10 @@
         <v>0.0266</v>
       </c>
       <c r="H31" t="n">
-        <v>16.35</v>
+        <v>14.4</v>
       </c>
       <c r="I31" t="n">
-        <v>0.021333</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="32">
@@ -1743,7 +1743,7 @@
         <v>20.2</v>
       </c>
       <c r="I35" t="n">
-        <v>0.014667</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="36">
@@ -1777,10 +1777,10 @@
         <v>0.0161</v>
       </c>
       <c r="H36" t="n">
-        <v>19.6</v>
+        <v>19.5</v>
       </c>
       <c r="I36" t="n">
-        <v>0.017</v>
+        <v>0.0175</v>
       </c>
     </row>
     <row r="37">
@@ -1814,10 +1814,10 @@
         <v>0.0137</v>
       </c>
       <c r="H37" t="n">
-        <v>12.65</v>
+        <v>14.3</v>
       </c>
       <c r="I37" t="n">
-        <v>0.02</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="38">
@@ -2073,7 +2073,7 @@
         <v>0.0032</v>
       </c>
       <c r="H44" t="n">
-        <v>12.4</v>
+        <v>13.9</v>
       </c>
       <c r="I44" t="n">
         <v>0.0135</v>
@@ -2295,7 +2295,7 @@
         <v>0.0069</v>
       </c>
       <c r="H50" t="n">
-        <v>9.85</v>
+        <v>12</v>
       </c>
       <c r="I50" t="n">
         <v>0.014</v>
@@ -2329,13 +2329,13 @@
         <v>7</v>
       </c>
       <c r="G51" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="H51" t="n">
-        <v>13.3</v>
+        <v>13.9</v>
       </c>
       <c r="I51" t="n">
-        <v>0.014</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="52">
@@ -2369,10 +2369,10 @@
         <v>0.014</v>
       </c>
       <c r="H52" t="n">
-        <v>17.65</v>
+        <v>17.8</v>
       </c>
       <c r="I52" t="n">
-        <v>0.0165</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="53">
@@ -2440,13 +2440,13 @@
         <v>7</v>
       </c>
       <c r="G54" t="n">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="H54" t="n">
         <v>19.9</v>
       </c>
       <c r="I54" t="n">
-        <v>0.0225</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="55">
@@ -2517,7 +2517,7 @@
         <v>0.021003</v>
       </c>
       <c r="H56" t="n">
-        <v>12.2</v>
+        <v>11.9</v>
       </c>
       <c r="I56" t="n">
         <v>0.027333</v>
@@ -2551,13 +2551,13 @@
         <v>7</v>
       </c>
       <c r="G57" t="n">
-        <v>0.01175</v>
+        <v>0.0045</v>
       </c>
       <c r="H57" t="n">
-        <v>17.15</v>
+        <v>17</v>
       </c>
       <c r="I57" t="n">
-        <v>0.0165</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="58">
@@ -2662,13 +2662,13 @@
         <v>7</v>
       </c>
       <c r="G60" t="n">
-        <v>0.015333</v>
+        <v>0.017</v>
       </c>
       <c r="H60" t="n">
         <v>21.5</v>
       </c>
       <c r="I60" t="n">
-        <v>0.0168</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="61">
@@ -2736,13 +2736,13 @@
         <v>7</v>
       </c>
       <c r="G62" t="n">
-        <v>0.00465</v>
+        <v>0.0047</v>
       </c>
       <c r="H62" t="n">
         <v>14.7</v>
       </c>
       <c r="I62" t="n">
-        <v>0.01375</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="63">
@@ -2776,10 +2776,10 @@
         <v>0.0046</v>
       </c>
       <c r="H63" t="n">
-        <v>16.425</v>
+        <v>16.733333</v>
       </c>
       <c r="I63" t="n">
-        <v>0.01375</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="64">
@@ -2813,7 +2813,7 @@
         <v>0.01102</v>
       </c>
       <c r="H64" t="n">
-        <v>18.628571</v>
+        <v>18.82</v>
       </c>
       <c r="I64" t="n">
         <v>0.0171</v>
@@ -2887,7 +2887,7 @@
         <v>0.0137</v>
       </c>
       <c r="H66" t="n">
-        <v>21</v>
+        <v>20.3</v>
       </c>
       <c r="I66" t="n">
         <v>0.018</v>
@@ -2924,7 +2924,7 @@
         <v>0.017</v>
       </c>
       <c r="H67" t="n">
-        <v>13.625</v>
+        <v>16.4</v>
       </c>
       <c r="I67" t="n">
         <v>0.022</v>
@@ -2998,10 +2998,10 @@
         <v>0.0037</v>
       </c>
       <c r="H69" t="n">
-        <v>17.733333</v>
+        <v>18.3</v>
       </c>
       <c r="I69" t="n">
-        <v>0.0156</v>
+        <v>0.01625</v>
       </c>
     </row>
     <row r="70">
@@ -3035,7 +3035,7 @@
         <v>0.0097</v>
       </c>
       <c r="H70" t="n">
-        <v>21.525</v>
+        <v>21.966667</v>
       </c>
       <c r="I70" t="n">
         <v>0.014333</v>
@@ -3072,10 +3072,10 @@
         <v>0.026</v>
       </c>
       <c r="H71" t="n">
-        <v>22.475</v>
+        <v>22.95</v>
       </c>
       <c r="I71" t="n">
-        <v>0.0176</v>
+        <v>0.016667</v>
       </c>
     </row>
     <row r="72">
@@ -3109,7 +3109,7 @@
         <v>0.019</v>
       </c>
       <c r="H72" t="n">
-        <v>18.7</v>
+        <v>17.9</v>
       </c>
       <c r="I72" t="n">
         <v>0.0225</v>
@@ -3149,7 +3149,7 @@
         <v>11.9</v>
       </c>
       <c r="I73" t="n">
-        <v>0.0274</v>
+        <v>0.028333</v>
       </c>
     </row>
     <row r="74">
@@ -3254,13 +3254,13 @@
         <v>7</v>
       </c>
       <c r="G76" t="n">
-        <v>0.039</v>
+        <v>0.053</v>
       </c>
       <c r="H76" t="n">
         <v>23.7</v>
       </c>
       <c r="I76" t="n">
-        <v>0.01625</v>
+        <v>0.0165</v>
       </c>
     </row>
     <row r="77">
@@ -3328,10 +3328,10 @@
         <v>7</v>
       </c>
       <c r="G78" t="n">
-        <v>0.030333</v>
+        <v>0.0315</v>
       </c>
       <c r="H78" t="n">
-        <v>19.933333</v>
+        <v>20.55</v>
       </c>
       <c r="I78" t="n">
         <v>0.02025</v>
@@ -3476,13 +3476,13 @@
         <v>7</v>
       </c>
       <c r="G82" t="n">
-        <v>0.01305</v>
+        <v>0.018</v>
       </c>
       <c r="H82" t="n">
         <v>17.8</v>
       </c>
       <c r="I82" t="n">
-        <v>0.0185</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="83">
@@ -3513,13 +3513,13 @@
         <v>7</v>
       </c>
       <c r="G83" t="n">
-        <v>0.0146</v>
+        <v>0.0245</v>
       </c>
       <c r="H83" t="n">
         <v>19.6</v>
       </c>
       <c r="I83" t="n">
-        <v>0.01825</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="84">
@@ -3550,7 +3550,7 @@
         <v>7</v>
       </c>
       <c r="G84" t="n">
-        <v>0.01405</v>
+        <v>0.019</v>
       </c>
       <c r="H84" t="n">
         <v>21.4</v>
@@ -3775,7 +3775,7 @@
         <v>0.022</v>
       </c>
       <c r="H90" t="n">
-        <v>19.35</v>
+        <v>18.5</v>
       </c>
       <c r="I90" t="n">
         <v>0.02</v>
@@ -3952,7 +3952,7 @@
         <v>0.00489</v>
       </c>
       <c r="H3" t="n">
-        <v>16.55</v>
+        <v>17.7</v>
       </c>
       <c r="I3" t="n">
         <v>0.0135</v>
@@ -4026,7 +4026,7 @@
         <v>0.01531</v>
       </c>
       <c r="H5" t="n">
-        <v>22.166667</v>
+        <v>21.5</v>
       </c>
       <c r="I5" t="n">
         <v>0.017</v>
@@ -4063,7 +4063,7 @@
         <v>0.0251</v>
       </c>
       <c r="H6" t="n">
-        <v>19.766667</v>
+        <v>20.8</v>
       </c>
       <c r="I6" t="n">
         <v>0.01925</v>
@@ -4100,7 +4100,7 @@
         <v>0.027003</v>
       </c>
       <c r="H7" t="n">
-        <v>18.11</v>
+        <v>19.28</v>
       </c>
       <c r="I7" t="n">
         <v>0.024438</v>
@@ -4208,13 +4208,13 @@
         <v>7</v>
       </c>
       <c r="G10" t="n">
-        <v>0.007425</v>
+        <v>0.00625</v>
       </c>
       <c r="H10" t="n">
         <v>20.3</v>
       </c>
       <c r="I10" t="n">
-        <v>0.019</v>
+        <v>0.0185</v>
       </c>
     </row>
     <row r="11">
@@ -4245,7 +4245,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01589</v>
+        <v>0.015887</v>
       </c>
       <c r="H11" t="n">
         <v>20.033333</v>
@@ -4282,7 +4282,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="n">
-        <v>0.004392</v>
+        <v>0.003802</v>
       </c>
       <c r="H12" t="n">
         <v>18.8</v>
@@ -4359,10 +4359,10 @@
         <v>0.007</v>
       </c>
       <c r="H14" t="n">
-        <v>12.25</v>
+        <v>13.5</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01975</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="15">
@@ -4396,10 +4396,10 @@
         <v>0.0046</v>
       </c>
       <c r="H15" t="n">
-        <v>16.45</v>
+        <v>18.1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.017333</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="16">
@@ -4470,7 +4470,7 @@
         <v>0.0207</v>
       </c>
       <c r="H17" t="n">
-        <v>20.733333</v>
+        <v>20.5</v>
       </c>
       <c r="I17" t="n">
         <v>0.016333</v>
@@ -4729,7 +4729,7 @@
         <v>0.0127</v>
       </c>
       <c r="H24" t="n">
-        <v>19.65</v>
+        <v>18.8</v>
       </c>
       <c r="I24" t="n">
         <v>0.017</v>
@@ -4951,10 +4951,10 @@
         <v>0.0318</v>
       </c>
       <c r="H30" t="n">
-        <v>19.8</v>
+        <v>20.4</v>
       </c>
       <c r="I30" t="n">
-        <v>0.018333</v>
+        <v>0.0185</v>
       </c>
     </row>
     <row r="31">
@@ -4988,10 +4988,10 @@
         <v>0.0266</v>
       </c>
       <c r="H31" t="n">
-        <v>16.35</v>
+        <v>14.4</v>
       </c>
       <c r="I31" t="n">
-        <v>0.021333</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="32">
@@ -5028,7 +5028,7 @@
         <v>9.699999999999999</v>
       </c>
       <c r="I32" t="n">
-        <v>0.013467</v>
+        <v>0.0119</v>
       </c>
     </row>
     <row r="33">
@@ -5139,7 +5139,7 @@
         <v>20.2</v>
       </c>
       <c r="I35" t="n">
-        <v>0.014667</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="36">
@@ -5173,10 +5173,10 @@
         <v>0.0161</v>
       </c>
       <c r="H36" t="n">
-        <v>19.6</v>
+        <v>19.5</v>
       </c>
       <c r="I36" t="n">
-        <v>0.017</v>
+        <v>0.0175</v>
       </c>
     </row>
     <row r="37">
@@ -5210,10 +5210,10 @@
         <v>0.0137</v>
       </c>
       <c r="H37" t="n">
-        <v>12.65</v>
+        <v>14.3</v>
       </c>
       <c r="I37" t="n">
-        <v>0.02</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="38">
@@ -5469,7 +5469,7 @@
         <v>0.0032</v>
       </c>
       <c r="H44" t="n">
-        <v>12.4</v>
+        <v>13.9</v>
       </c>
       <c r="I44" t="n">
         <v>0.0135</v>
@@ -5617,7 +5617,7 @@
         <v>0.018956</v>
       </c>
       <c r="H48" t="n">
-        <v>18.974742</v>
+        <v>18.742784</v>
       </c>
       <c r="I48" t="n">
         <v>0.019307</v>
@@ -5691,7 +5691,7 @@
         <v>0.0069</v>
       </c>
       <c r="H50" t="n">
-        <v>9.85</v>
+        <v>12</v>
       </c>
       <c r="I50" t="n">
         <v>0.014</v>
@@ -5725,13 +5725,13 @@
         <v>7</v>
       </c>
       <c r="G51" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="H51" t="n">
-        <v>13.3</v>
+        <v>13.9</v>
       </c>
       <c r="I51" t="n">
-        <v>0.014</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="52">
@@ -5765,10 +5765,10 @@
         <v>0.014</v>
       </c>
       <c r="H52" t="n">
-        <v>17.65</v>
+        <v>17.8</v>
       </c>
       <c r="I52" t="n">
-        <v>0.0165</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="53">
@@ -5836,13 +5836,13 @@
         <v>7</v>
       </c>
       <c r="G54" t="n">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="H54" t="n">
         <v>19.9</v>
       </c>
       <c r="I54" t="n">
-        <v>0.0225</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="55">
@@ -5876,7 +5876,7 @@
         <v>0.022</v>
       </c>
       <c r="H55" t="n">
-        <v>19.63</v>
+        <v>20.44</v>
       </c>
       <c r="I55" t="n">
         <v>0.02075</v>
@@ -5913,7 +5913,7 @@
         <v>0.021003</v>
       </c>
       <c r="H56" t="n">
-        <v>11.45</v>
+        <v>11.1125</v>
       </c>
       <c r="I56" t="n">
         <v>0.027333</v>
@@ -5947,13 +5947,13 @@
         <v>7</v>
       </c>
       <c r="G57" t="n">
-        <v>0.01175</v>
+        <v>0.0045</v>
       </c>
       <c r="H57" t="n">
-        <v>17.15</v>
+        <v>17</v>
       </c>
       <c r="I57" t="n">
-        <v>0.0165</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="58">
@@ -6058,13 +6058,13 @@
         <v>7</v>
       </c>
       <c r="G60" t="n">
-        <v>0.015333</v>
+        <v>0.017</v>
       </c>
       <c r="H60" t="n">
         <v>21.5</v>
       </c>
       <c r="I60" t="n">
-        <v>0.0168</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="61">
@@ -6098,7 +6098,7 @@
         <v>0.018</v>
       </c>
       <c r="H61" t="n">
-        <v>17.6</v>
+        <v>17.4875</v>
       </c>
       <c r="I61" t="n">
         <v>0.018</v>
@@ -6132,13 +6132,13 @@
         <v>7</v>
       </c>
       <c r="G62" t="n">
-        <v>0.00465</v>
+        <v>0.0047</v>
       </c>
       <c r="H62" t="n">
         <v>14.7</v>
       </c>
       <c r="I62" t="n">
-        <v>0.01375</v>
+        <v>0.0145</v>
       </c>
     </row>
     <row r="63">
@@ -6172,10 +6172,10 @@
         <v>0.0046</v>
       </c>
       <c r="H63" t="n">
-        <v>16.425</v>
+        <v>16.733333</v>
       </c>
       <c r="I63" t="n">
-        <v>0.01375</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="64">
@@ -6209,7 +6209,7 @@
         <v>0.01102</v>
       </c>
       <c r="H64" t="n">
-        <v>18.628571</v>
+        <v>18.82</v>
       </c>
       <c r="I64" t="n">
         <v>0.0171</v>
@@ -6283,7 +6283,7 @@
         <v>0.0137</v>
       </c>
       <c r="H66" t="n">
-        <v>21</v>
+        <v>20.3</v>
       </c>
       <c r="I66" t="n">
         <v>0.018</v>
@@ -6320,7 +6320,7 @@
         <v>0.017</v>
       </c>
       <c r="H67" t="n">
-        <v>13.625</v>
+        <v>16.4</v>
       </c>
       <c r="I67" t="n">
         <v>0.022</v>
@@ -6394,10 +6394,10 @@
         <v>0.0037</v>
       </c>
       <c r="H69" t="n">
-        <v>17.733333</v>
+        <v>18.3</v>
       </c>
       <c r="I69" t="n">
-        <v>0.0156</v>
+        <v>0.01625</v>
       </c>
     </row>
     <row r="70">
@@ -6431,7 +6431,7 @@
         <v>0.0097</v>
       </c>
       <c r="H70" t="n">
-        <v>21.525</v>
+        <v>21.966667</v>
       </c>
       <c r="I70" t="n">
         <v>0.014333</v>
@@ -6468,10 +6468,10 @@
         <v>0.026</v>
       </c>
       <c r="H71" t="n">
-        <v>22.475</v>
+        <v>22.95</v>
       </c>
       <c r="I71" t="n">
-        <v>0.0176</v>
+        <v>0.016667</v>
       </c>
     </row>
     <row r="72">
@@ -6505,7 +6505,7 @@
         <v>0.019</v>
       </c>
       <c r="H72" t="n">
-        <v>18.7</v>
+        <v>17.9</v>
       </c>
       <c r="I72" t="n">
         <v>0.0225</v>
@@ -6545,7 +6545,7 @@
         <v>11.9</v>
       </c>
       <c r="I73" t="n">
-        <v>0.028973</v>
+        <v>0.028583</v>
       </c>
     </row>
     <row r="74">
@@ -6576,7 +6576,7 @@
         <v>7</v>
       </c>
       <c r="G74" t="n">
-        <v>0.020467</v>
+        <v>0.02735</v>
       </c>
       <c r="H74" t="n">
         <v>10.9</v>
@@ -6650,13 +6650,13 @@
         <v>7</v>
       </c>
       <c r="G76" t="n">
-        <v>0.039</v>
+        <v>0.053</v>
       </c>
       <c r="H76" t="n">
         <v>23.7</v>
       </c>
       <c r="I76" t="n">
-        <v>0.01625</v>
+        <v>0.0165</v>
       </c>
     </row>
     <row r="77">
@@ -6724,10 +6724,10 @@
         <v>7</v>
       </c>
       <c r="G78" t="n">
-        <v>0.030333</v>
+        <v>0.0315</v>
       </c>
       <c r="H78" t="n">
-        <v>19.933333</v>
+        <v>20.55</v>
       </c>
       <c r="I78" t="n">
         <v>0.02025</v>
@@ -6767,7 +6767,7 @@
         <v>16.7</v>
       </c>
       <c r="I79" t="n">
-        <v>0.0233</v>
+        <v>0.0231</v>
       </c>
     </row>
     <row r="80">
@@ -6872,13 +6872,13 @@
         <v>7</v>
       </c>
       <c r="G82" t="n">
-        <v>0.01305</v>
+        <v>0.018</v>
       </c>
       <c r="H82" t="n">
         <v>17.8</v>
       </c>
       <c r="I82" t="n">
-        <v>0.0185</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="83">
@@ -6909,13 +6909,13 @@
         <v>7</v>
       </c>
       <c r="G83" t="n">
-        <v>0.012334</v>
+        <v>0.013571</v>
       </c>
       <c r="H83" t="n">
         <v>20.209091</v>
       </c>
       <c r="I83" t="n">
-        <v>0.01875</v>
+        <v>0.017386</v>
       </c>
     </row>
     <row r="84">
@@ -6946,7 +6946,7 @@
         <v>7</v>
       </c>
       <c r="G84" t="n">
-        <v>0.013405</v>
+        <v>0.014643</v>
       </c>
       <c r="H84" t="n">
         <v>21.4</v>
@@ -7171,7 +7171,7 @@
         <v>0.022</v>
       </c>
       <c r="H90" t="n">
-        <v>19.35</v>
+        <v>18.5</v>
       </c>
       <c r="I90" t="n">
         <v>0.02</v>

</xml_diff>